<commit_message>
finished extracting the data
</commit_message>
<xml_diff>
--- a/ML/ML_files/2014_APRIL.xlsx
+++ b/ML/ML_files/2014_APRIL.xlsx
@@ -4285,7 +4285,7 @@
         <v>4665</v>
       </c>
       <c r="J72">
-        <v>72.17577706323686</v>
+        <v>72.17577706323687</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -4331,7 +4331,7 @@
         <v>2871</v>
       </c>
       <c r="G73">
-        <v>97.70114942528735</v>
+        <v>97.70114942528736</v>
       </c>
       <c r="H73">
         <v>5315</v>
@@ -4866,7 +4866,7 @@
         <v>7230506</v>
       </c>
       <c r="D83">
-        <v>-20.90985056924094</v>
+        <v>-20.90985056924095</v>
       </c>
       <c r="E83">
         <v>1798673</v>
@@ -6021,7 +6021,7 @@
         <v>1264357</v>
       </c>
       <c r="G104">
-        <v>-53.80466118351067</v>
+        <v>-53.80466118351068</v>
       </c>
       <c r="H104">
         <v>2177673</v>
@@ -6284,7 +6284,7 @@
         <v>1700857</v>
       </c>
       <c r="G109">
-        <v>-42.20736957898283</v>
+        <v>-42.20736957898284</v>
       </c>
       <c r="H109">
         <v>2194064</v>
@@ -6357,7 +6357,7 @@
         <v>237030</v>
       </c>
       <c r="M110">
-        <v>-22.61232755347424</v>
+        <v>-22.61232755347425</v>
       </c>
       <c r="N110">
         <v>209</v>
@@ -6539,7 +6539,7 @@
         <v>265328</v>
       </c>
       <c r="M115">
-        <v>149.5835343423988</v>
+        <v>149.5835343423989</v>
       </c>
       <c r="N115">
         <v>373</v>
@@ -7013,7 +7013,7 @@
         <v>674500</v>
       </c>
       <c r="M124">
-        <v>-32.18680504077093</v>
+        <v>-32.18680504077094</v>
       </c>
       <c r="N124">
         <v>230</v>
@@ -7215,7 +7215,7 @@
         <v>55322</v>
       </c>
       <c r="G128">
-        <v>-74.61407758215537</v>
+        <v>-74.61407758215538</v>
       </c>
       <c r="H128">
         <v>80032</v>
@@ -8040,7 +8040,7 @@
         <v>505028</v>
       </c>
       <c r="J143">
-        <v>36.1086910032711</v>
+        <v>36.10869100327111</v>
       </c>
       <c r="K143">
         <v>585980</v>
@@ -8306,7 +8306,7 @@
         <v>1213</v>
       </c>
       <c r="G148">
-        <v>496.2077493816982</v>
+        <v>496.2077493816983</v>
       </c>
       <c r="H148">
         <v>16393</v>
@@ -8462,7 +8462,7 @@
         <v>12508</v>
       </c>
       <c r="D151">
-        <v>-46.25839462743843</v>
+        <v>-46.25839462743844</v>
       </c>
       <c r="E151">
         <v>3854</v>

</xml_diff>